<commit_message>
update multi search, search 3d
</commit_message>
<xml_diff>
--- a/outputs/arxiv_report_0709_0716.xlsx
+++ b/outputs/arxiv_report_0709_0716.xlsx
@@ -7,11 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Architecture" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Embodied AI" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LLM Other Compression" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LLM Pruning" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LLM Quantization" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3D" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Architecture" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Embodied AI" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LLM Compression Others" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LLM Pruning" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LLM Quantization" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,6 +430,670 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>更新日期</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>发表日期</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>文章标题</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>匹配关键词</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>作者</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>摘要</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2024-12-11</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SLGaussian: Fast Language Gaussian Splatting in Sparse Views</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>3DGS</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Kangjie Chen, BingQuan Dai, Minghan Qin, Dongbin Zhang, Peihao Li, Yingshuang Zou, Haoqian Wang</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2412.08331v2</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>3D semantic field learning is crucial for applications like autonomous
+navigation, AR/VR, and robotics, where accurate comprehension of 3D scenes from
+limited viewpoints is essential. Existing methods struggle under sparse view
+conditions, relying on inefficient per-scene multi-view optimizations, which
+are impractical for many real-world tasks. To address this, we propose
+SLGaussian, a feed-forward method for constructing 3D semantic fields from
+sparse viewpoints, allowing direct inference of 3DGS-based scenes. By ensuring
+consistent SAM segmentations through video tracking and using low-dimensional
+indexing for high-dimensional CLIP features, SLGaussian efficiently embeds
+language information in 3D space, offering a robust solution for accurate 3D
+scene understanding under sparse view conditions. In experiments on two-view
+sparse 3D object querying and segmentation in the LERF and 3D-OVS datasets,
+SLGaussian outperforms existing methods in chosen IoU, Localization Accuracy,
+and mIoU. Moreover, our model achieves scene inference in under 30 seconds and
+open-vocabulary querying in just 0.011 seconds per query.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CoMoGaussian: Continuous Motion-Aware Gaussian Splatting from Motion-Blurred Images</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3DGS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Jungho Lee, Donghyeong Kim, Dogyoon Lee, Suhwan Cho, Minhyeok Lee, Wonjoon Lee, Taeoh Kim, Dongyoon Wee, Sangyoun Lee</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2503.05332v2</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>3D Gaussian Splatting (3DGS) has gained significant attention due to its
+high-quality novel view rendering, motivating research to address real-world
+challenges. A critical issue is the camera motion blur caused by movement
+during exposure, which hinders accurate 3D scene reconstruction. In this study,
+we propose CoMoGaussian, a Continuous Motion-Aware Gaussian Splatting that
+reconstructs precise 3D scenes from motion-blurred images while maintaining
+real-time rendering speed. Considering the complex motion patterns inherent in
+real-world camera movements, we predict continuous camera trajectories using
+neural ordinary differential equations (ODEs). To ensure accurate modeling, we
+employ rigid body transformations, preserving the shape and size of the object
+but rely on the discrete integration of sampled frames. To better approximate
+the continuous nature of motion blur, we introduce a continuous motion
+refinement (CMR) transformation that refines rigid transformations by
+incorporating additional learnable parameters. By revisiting fundamental camera
+theory and leveraging advanced neural ODE techniques, we achieve precise
+modeling of continuous camera trajectories, leading to improved reconstruction
+accuracy. Extensive experiments demonstrate state-of-the-art performance both
+quantitatively and qualitatively on benchmark datasets, which include a wide
+range of motion blur scenarios, from moderate to extreme blur.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>HGSLoc: 3DGS-based Heuristic Camera Pose Refinement</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NeRF, Neural Rendering</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Zhongyan Niu, Zhen Tan, Jinpu Zhang, Xueliang Yang, Dewen Hu</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2409.10925v3</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Visual localization refers to the process of determining camera poses and
+orientation within a known scene representation. This task is often complicated
+by factors such as changes in illumination and variations in viewing angles. In
+this paper, we propose HGSLoc, a novel lightweight plug-and-play pose
+optimization framework, which integrates 3D reconstruction with a heuristic
+refinement strategy to achieve higher pose estimation accuracy. Specifically,
+we introduce an explicit geometric map for 3D representation and high-fidelity
+rendering, allowing the generation of high-quality synthesized views to support
+accurate visual localization. Our method demonstrates higher localization
+accuracy compared to NeRF-based neural rendering localization approaches. We
+introduce a heuristic refinement strategy, its efficient optimization
+capability can quickly locate the target node, while we set the step level
+optimization step to enhance the pose accuracy in the scenarios with small
+errors. With carefully designed heuristic functions, it offers efficient
+optimization capabilities, enabling rapid error reduction in rough localization
+estimations. Our method mitigates the dependence on complex neural network
+models while demonstrating improved robustness against noise and higher
+localization accuracy in challenging environments, as compared to neural
+network joint optimization strategies. The optimization framework proposed in
+this paper introduces novel approaches to visual localization by integrating
+the advantages of 3D reconstruction and the heuristic refinement strategy,
+which demonstrates strong performance across multiple benchmark datasets,
+including 7Scenes and Deep Blending dataset. The implementation of our method
+has been released at https://github.com/anchang699/HGSLoc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3DGAA: Realistic and Robust 3D Gaussian-based Adversarial Attack for Autonomous Driving</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3DGS</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Yixun Zhang, Lizhi Wang, Junjun Zhao, Wending Zhao, Feng Zhou, Yonghao Dang, Jianqin Yin</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2507.09993v1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Camera-based object detection systems play a vital role in autonomous
+driving, yet they remain vulnerable to adversarial threats in real-world
+environments. While existing 2D and 3D physical attacks typically optimize
+texture, they often struggle to balance physical realism and attack robustness.
+In this work, we propose 3D Gaussian-based Adversarial Attack (3DGAA), a novel
+adversarial object generation framework that leverages the full 14-dimensional
+parameterization of 3D Gaussian Splatting (3DGS) to jointly optimize geometry
+and appearance in physically realizable ways. Unlike prior works that rely on
+patches or texture, 3DGAA jointly perturbs both geometric attributes (shape,
+scale, rotation) and appearance attributes (color, opacity) to produce
+physically realistic and transferable adversarial objects. We further introduce
+a physical filtering module to preserve geometric fidelity, and a physical
+augmentation module to simulate complex physical scenarios, thus enhancing
+attack generalization under real-world conditions. We evaluate 3DGAA on both
+virtual benchmarks and physical-world setups using miniature vehicle models.
+Experimental results show that 3DGAA achieves to reduce the detection mAP from
+87.21% to 7.38%, significantly outperforming existing 3D physical attacks.
+Moreover, our method maintains high transferability across different physical
+conditions, demonstrating a new state-of-the-art in physically realizable
+adversarial attacks. These results validate 3DGAA as a practical attack
+framework for evaluating the safety of perception systems in autonomous
+driving.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-07-14</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CLiFT: Compressive Light-Field Tokens for Compute-Efficient and Adaptive Neural Rendering</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Neural Rendering</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Zhengqing Wang, Yuefan Wu, Jiacheng Chen, Fuyang Zhang, Yasutaka Furukawa</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2507.08776v2</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>This paper proposes a neural rendering approach that represents a scene as
+"compressed light-field tokens (CLiFTs)", retaining rich appearance and
+geometric information of a scene. CLiFT enables compute-efficient rendering by
+compressed tokens, while being capable of changing the number of tokens to
+represent a scene or render a novel view with one trained network. Concretely,
+given a set of images, multi-view encoder tokenizes the images with the camera
+poses. Latent-space K-means selects a reduced set of rays as cluster centroids
+using the tokens. The multi-view ``condenser'' compresses the information of
+all the tokens into the centroid tokens to construct CLiFTs. At test time,
+given a target view and a compute budget (i.e., the number of CLiFTs), the
+system collects the specified number of nearby tokens and synthesizes a novel
+view using a compute-adaptive renderer. Extensive experiments on RealEstate10K
+and DL3DV datasets quantitatively and qualitatively validate our approach,
+achieving significant data reduction with comparable rendering quality and the
+highest overall rendering score, while providing trade-offs of data size,
+rendering quality, and rendering speed.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-07-12</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Stable Score Distillation</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NeRF</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Haiming Zhu, Yangyang Xu, Chenshu Xu, Tingrui Shen, Wenxi Liu, Yong Du, Jun Yu, Shengfeng He</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2507.09168v1</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Text-guided image and 3D editing have advanced with diffusion-based models,
+yet methods like Delta Denoising Score often struggle with stability, spatial
+control, and editing strength. These limitations stem from reliance on complex
+auxiliary structures, which introduce conflicting optimization signals and
+restrict precise, localized edits. We introduce Stable Score Distillation
+(SSD), a streamlined framework that enhances stability and alignment in the
+editing process by anchoring a single classifier to the source prompt.
+Specifically, SSD utilizes Classifier-Free Guidance (CFG) equation to achieves
+cross-prompt alignment, and introduces a constant term null-text branch to
+stabilize the optimization process. This approach preserves the original
+content's structure and ensures that editing trajectories are closely aligned
+with the source prompt, enabling smooth, prompt-specific modifications while
+maintaining coherence in surrounding regions. Additionally, SSD incorporates a
+prompt enhancement branch to boost editing strength, particularly for style
+transformations. Our method achieves state-of-the-art results in 2D and 3D
+editing tasks, including NeRF and text-driven style edits, with faster
+convergence and reduced complexity, providing a robust and efficient solution
+for text-guided editing.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>From images to properties: a NeRF-driven framework for granular material parameter inversion</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NeRF</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Cheng-Hsi Hsiao, Krishna Kumar</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2507.09005v1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>We introduce a novel framework that integrates Neural Radiance Fields (NeRF)
+with Material Point Method (MPM) simulation to infer granular material
+properties from visual observations. Our approach begins by generating
+synthetic experimental data, simulating an plow interacting with sand. The
+experiment is rendered into realistic images as the photographic observations.
+These observations include multi-view images of the experiment's initial state
+and time-sequenced images from two fixed cameras. Using NeRF, we reconstruct
+the 3D geometry from the initial multi-view images, leveraging its capability
+to synthesize novel viewpoints and capture intricate surface details. The
+reconstructed geometry is then used to initialize material point positions for
+the MPM simulation, where the friction angle remains unknown. We render images
+of the simulation under the same camera setup and compare them to the observed
+images. By employing Bayesian optimization, we minimize the image loss to
+estimate the best-fitting friction angle. Our results demonstrate that friction
+angle can be estimated with an error within 2 degrees, highlighting the
+effectiveness of inverse analysis through purely visual observations. This
+approach offers a promising solution for characterizing granular materials in
+real-world scenarios where direct measurement is impractical or impossible.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-07-11</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-10-31</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>GeoSplatting: Towards Geometry Guided Gaussian Splatting for Physically-based Inverse Rendering</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3DGS</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Kai Ye, Chong Gao, Guanbin Li, Wenzheng Chen, Baoquan Chen</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2410.24204v3</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Recent 3D Gaussian Splatting (3DGS) representations have demonstrated
+remarkable performance in novel view synthesis; further, material-lighting
+disentanglement on 3DGS warrants relighting capabilities and its adaptability
+to broader applications. While the general approach to the latter operation
+lies in integrating differentiable physically-based rendering (PBR) techniques
+to jointly recover BRDF materials and environment lighting, achieving a precise
+disentanglement remains an inherently difficult task due to the challenge of
+accurately modeling light transport. Existing approaches typically approximate
+Gaussian points' normals, which constitute an implicit geometric constraint.
+However, they usually suffer from inaccuracies in normal estimation that
+subsequently degrade light transport, resulting in noisy material decomposition
+and flawed relighting results. To address this, we propose GeoSplatting, a
+novel approach that augments 3DGS with explicit geometry guidance for precise
+light transport modeling. By differentiably constructing a surface-grounded
+3DGS from an optimizable mesh, our approach leverages well-defined mesh normals
+and the opaque mesh surface, and additionally facilitates the use of mesh-based
+ray tracing techniques for efficient, occlusion-aware light transport
+calculations. This enhancement ensures precise material decomposition while
+preserving the efficiency and high-quality rendering capabilities of 3DGS.
+Comprehensive evaluations across diverse datasets demonstrate the effectiveness
+of GeoSplatting, highlighting its superior efficiency and state-of-the-art
+inverse rendering performance. The project page can be found at
+https://pku-vcl-geometry.github.io/GeoSplatting/.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>RegGS: Unposed Sparse Views Gaussian Splatting with 3DGS Registration</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3DGS</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Chong Cheng, Yu Hu, Sicheng Yu, Beizhen Zhao, Zijian Wang, Hao Wang</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2507.08136v1</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>3D Gaussian Splatting (3DGS) has demonstrated its potential in reconstructing
+scenes from unposed images. However, optimization-based 3DGS methods struggle
+with sparse views due to limited prior knowledge. Meanwhile, feed-forward
+Gaussian approaches are constrained by input formats, making it challenging to
+incorporate more input views. To address these challenges, we propose RegGS, a
+3D Gaussian registration-based framework for reconstructing unposed sparse
+views. RegGS aligns local 3D Gaussians generated by a feed-forward network into
+a globally consistent 3D Gaussian representation. Technically, we implement an
+entropy-regularized Sinkhorn algorithm to efficiently solve the optimal
+transport Mixture 2-Wasserstein $(\text{MW}_2)$ distance, which serves as an
+alignment metric for Gaussian mixture models (GMMs) in $\mathrm{Sim}(3)$ space.
+Furthermore, we design a joint 3DGS registration module that integrates the
+$\text{MW}_2$ distance, photometric consistency, and depth geometry. This
+enables a coarse-to-fine registration process while accurately estimating
+camera poses and aligning the scene. Experiments on the RE10K and ACID datasets
+demonstrate that RegGS effectively registers local Gaussians with high
+fidelity, achieving precise pose estimation and high-quality novel-view
+synthesis. Project page: https://3dagentworld.github.io/reggs/.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>RTR-GS: 3D Gaussian Splatting for Inverse Rendering with Radiance Transfer and Reflection</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>3DGS</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Yongyang Zhou, Fang-Lue Zhang, Zichen Wang, Lei Zhang</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2507.07733v1</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>3D Gaussian Splatting (3DGS) has demonstrated impressive capabilities in
+novel view synthesis. However, rendering reflective objects remains a
+significant challenge, particularly in inverse rendering and relighting. We
+introduce RTR-GS, a novel inverse rendering framework capable of robustly
+rendering objects with arbitrary reflectance properties, decomposing BRDF and
+lighting, and delivering credible relighting results. Given a collection of
+multi-view images, our method effectively recovers geometric structure through
+a hybrid rendering model that combines forward rendering for radiance transfer
+with deferred rendering for reflections. This approach successfully separates
+high-frequency and low-frequency appearances, mitigating floating artifacts
+caused by spherical harmonic overfitting when handling high-frequency details.
+We further refine BRDF and lighting decomposition using an additional
+physically-based deferred rendering branch. Experimental results show that our
+method enhances novel view synthesis, normal estimation, decomposition, and
+relighting while maintaining efficient training inference process.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MUVOD: A Novel Multi-view Video Object Segmentation Dataset and A Benchmark for 3D Segmentation</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>NeRF</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bangning Wei, Joshua Maraval, Meriem Outtas, Kidiyo Kpalma, Nicolas Ramin, Lu Zhang</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>http://arxiv.org/abs/2507.07519v1</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>The application of methods based on Neural Radiance Fields (NeRF) and 3D
+Gaussian Splatting (3D GS) have steadily gained popularity in the field of 3D
+object segmentation in static scenes. These approaches demonstrate efficacy in
+a range of 3D scene understanding and editing tasks. Nevertheless, the 4D
+object segmentation of dynamic scenes remains an underexplored field due to the
+absence of a sufficiently extensive and accurately labelled multi-view video
+dataset. In this paper, we present MUVOD, a new multi-view video dataset for
+training and evaluating object segmentation in reconstructed real-world
+scenarios. The 17 selected scenes, describing various indoor or outdoor
+activities, are collected from different sources of datasets originating from
+various types of camera rigs. Each scene contains a minimum of 9 views and a
+maximum of 46 views. We provide 7830 RGB images (30 frames per video) with
+their corresponding segmentation mask in 4D motion, meaning that any object of
+interest in the scene could be tracked across temporal frames of a given view
+or across different views belonging to the same camera rig. This dataset, which
+contains 459 instances of 73 categories, is intended as a basic benchmark for
+the evaluation of multi-view video segmentation methods. We also present an
+evaluation metric and a baseline segmentation approach to encourage and
+evaluate progress in this evolving field. Additionally, we propose a new
+benchmark for 3D object segmentation task with a subset of annotated multi-view
+images selected from our MUVOD dataset. This subset contains 50 objects of
+different conditions in different scenarios, providing a more comprehensive
+analysis of state-of-the-art 3D object segmentation methods. Our proposed MUVOD
+dataset is available at https://volumetric-repository.labs.b-com.com/#/muvod.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1746,7 +2411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2576,7 +3241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3179,7 +3844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4546,7 +5211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>